<commit_message>
Upload file 4duk_channels on 2023-10-17 14:18:36.700180
</commit_message>
<xml_diff>
--- a/4duk_channels.xlsx
+++ b/4duk_channels.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C439"/>
+  <dimension ref="A1:C434"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1687,7 +1687,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Киноужас HD</t>
+          <t>К-Ужас HD</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -2758,7 +2758,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>Paramount Comedy</t>
+          <t>Comedy Central</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
@@ -2826,7 +2826,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Кинопремьера HD</t>
+          <t>К-Премьера HD</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
@@ -2860,7 +2860,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Киносвидание HD</t>
+          <t>К-Свидание HD</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
@@ -2911,7 +2911,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Киносемья HD</t>
+          <t>К-Семья HD</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
@@ -3064,12 +3064,12 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>TV3 Film HD</t>
+          <t>Блокбастер HD</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>13000919</t>
+          <t>13000849</t>
         </is>
       </c>
     </row>
@@ -3081,12 +3081,12 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Блокбастер HD</t>
+          <t>KinoJam 1 HD</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>13000849</t>
+          <t>13000920</t>
         </is>
       </c>
     </row>
@@ -3098,12 +3098,12 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>KinoJam 1 HD</t>
+          <t>FlixSnip HD</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>13000920</t>
+          <t>13000850</t>
         </is>
       </c>
     </row>
@@ -3115,12 +3115,12 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>FlixSnip HD</t>
+          <t>KinoJam 2 HD</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>13000850</t>
+          <t>13000921</t>
         </is>
       </c>
     </row>
@@ -3132,12 +3132,12 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>KinoJam 2 HD</t>
+          <t>VIP Comedy HD</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>13000921</t>
+          <t>13000744</t>
         </is>
       </c>
     </row>
@@ -3149,12 +3149,12 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>VIP Comedy HD</t>
+          <t>Комедия</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>13000744</t>
+          <t>13000930</t>
         </is>
       </c>
     </row>
@@ -3166,12 +3166,12 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Комедия</t>
+          <t>VIP Megahit HD</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>13000930</t>
+          <t>13000745</t>
         </is>
       </c>
     </row>
@@ -3183,12 +3183,12 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>VIP Megahit HD</t>
+          <t>Кинопоказ HD</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>13000745</t>
+          <t>13000854</t>
         </is>
       </c>
     </row>
@@ -3200,12 +3200,12 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Кинопоказ HD</t>
+          <t>VIP Premiere HD</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>13000854</t>
+          <t>13000746</t>
         </is>
       </c>
     </row>
@@ -3217,12 +3217,12 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>VIP Premiere HD</t>
+          <t>VIP Serial HD</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>13000746</t>
+          <t>13000743</t>
         </is>
       </c>
     </row>
@@ -3234,12 +3234,12 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>VIP Serial HD</t>
+          <t>Киноман</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>13000743</t>
+          <t>13000853</t>
         </is>
       </c>
     </row>
@@ -3251,12 +3251,12 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Киноман</t>
+          <t>Про100ТВ</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>13000853</t>
+          <t>13000996</t>
         </is>
       </c>
     </row>
@@ -3268,12 +3268,12 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Про100ТВ</t>
+          <t>Победа HD</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>13000996</t>
+          <t>13000747</t>
         </is>
       </c>
     </row>
@@ -3285,12 +3285,12 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Победа HD</t>
+          <t>Советское кино</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>13000747</t>
+          <t>13000810</t>
         </is>
       </c>
     </row>
@@ -3302,12 +3302,12 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Советское кино</t>
+          <t>Кино ТВ HD</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>13000810</t>
+          <t>13000748</t>
         </is>
       </c>
     </row>
@@ -3319,12 +3319,12 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Кино ТВ HD</t>
+          <t>День Победы HD</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>13000748</t>
+          <t>13000856</t>
         </is>
       </c>
     </row>
@@ -3336,12 +3336,12 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>День Победы HD</t>
+          <t>VB Спецназ-Диверсант</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>13000856</t>
+          <t>13001185</t>
         </is>
       </c>
     </row>
@@ -3353,12 +3353,12 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>VB Спецназ-Диверсант</t>
+          <t>Мир сериала</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>13001185</t>
+          <t>13000870</t>
         </is>
       </c>
     </row>
@@ -3370,12 +3370,12 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Мир сериала</t>
+          <t>Твоё ТВ HD</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>13000870</t>
+          <t>13000618</t>
         </is>
       </c>
     </row>
@@ -3387,12 +3387,12 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Твоё ТВ HD</t>
+          <t>Discovery HD</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>13000618</t>
+          <t>13000749</t>
         </is>
       </c>
     </row>
@@ -3404,12 +3404,12 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Discovery HD</t>
+          <t>Discovery Science HD</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>13000749</t>
+          <t>13000752</t>
         </is>
       </c>
     </row>
@@ -3421,12 +3421,12 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Discovery Science HD</t>
+          <t>English Club TV HD</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>13000752</t>
+          <t>13000751</t>
         </is>
       </c>
     </row>
@@ -3438,12 +3438,12 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>English Club TV HD</t>
+          <t>History HD</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>13000751</t>
+          <t>13000753</t>
         </is>
       </c>
     </row>
@@ -3455,12 +3455,12 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>History HD</t>
+          <t>H2 HD</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>13000753</t>
+          <t>13000754</t>
         </is>
       </c>
     </row>
@@ -3472,12 +3472,12 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>H2 HD</t>
+          <t>ID Xtra HD</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>13000754</t>
+          <t>13000755</t>
         </is>
       </c>
     </row>
@@ -3489,12 +3489,12 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>ID Xtra HD</t>
+          <t>National Geographic HD</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>13000755</t>
+          <t>13000756</t>
         </is>
       </c>
     </row>
@@ -3506,12 +3506,12 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>National Geographic HD</t>
+          <t>Nat Geo Wild HD</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>13000756</t>
+          <t>13000214</t>
         </is>
       </c>
     </row>
@@ -3523,12 +3523,12 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Nat Geo Wild HD</t>
+          <t>Animal Planet HD</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>13000214</t>
+          <t>13000806</t>
         </is>
       </c>
     </row>
@@ -3540,12 +3540,12 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Animal Planet HD</t>
+          <t>RTG HD</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>13000806</t>
+          <t>13000757</t>
         </is>
       </c>
     </row>
@@ -3557,12 +3557,12 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>RTG HD</t>
+          <t>Арсенал HD</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>13000757</t>
+          <t>13000863</t>
         </is>
       </c>
     </row>
@@ -3574,12 +3574,12 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Арсенал HD</t>
+          <t>Viasat Explore HD</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>13000863</t>
+          <t>13000760</t>
         </is>
       </c>
     </row>
@@ -3591,12 +3591,12 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Viasat Explore HD</t>
+          <t>Viasat History HD</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>13000760</t>
+          <t>13000761</t>
         </is>
       </c>
     </row>
@@ -3608,12 +3608,12 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Viasat History HD</t>
+          <t>RT Doc HD</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>13000761</t>
+          <t>13000868</t>
         </is>
       </c>
     </row>
@@ -3625,12 +3625,12 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>RT Doc HD</t>
+          <t>Viasat Nature HD</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>13000868</t>
+          <t>13000762</t>
         </is>
       </c>
     </row>
@@ -3642,12 +3642,12 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Viasat Nature HD</t>
+          <t>Viasat Nature/History HD</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>13000762</t>
+          <t>13000763</t>
         </is>
       </c>
     </row>
@@ -3659,12 +3659,12 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>Viasat Nature/History HD</t>
+          <t>Ocean TV</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>13000763</t>
+          <t>13000793</t>
         </is>
       </c>
     </row>
@@ -3676,12 +3676,12 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>Ocean TV</t>
+          <t>Большая Азия HD</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>13000793</t>
+          <t>13000769</t>
         </is>
       </c>
     </row>
@@ -3693,12 +3693,12 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>Большая Азия HD</t>
+          <t>Первый Космический HD</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>13000769</t>
+          <t>13000612</t>
         </is>
       </c>
     </row>
@@ -3710,12 +3710,12 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Первый Космический HD</t>
+          <t>Живая планета</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>13000612</t>
+          <t>13000794</t>
         </is>
       </c>
     </row>
@@ -3727,12 +3727,12 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>Живая планета</t>
+          <t>HDL</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>13000794</t>
+          <t>13000807</t>
         </is>
       </c>
     </row>
@@ -3744,12 +3744,12 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>HDL</t>
+          <t>Еда Премиум HD</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>13000807</t>
+          <t>13000764</t>
         </is>
       </c>
     </row>
@@ -3761,12 +3761,12 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>Еда Премиум HD</t>
+          <t>А-24 HD</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>13000764</t>
+          <t>13000765</t>
         </is>
       </c>
     </row>
@@ -3778,12 +3778,12 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>АВТО24 HD</t>
+          <t>Зал суда HD</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>13000765</t>
+          <t>13000707</t>
         </is>
       </c>
     </row>
@@ -3795,12 +3795,12 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>Зал суда HD</t>
+          <t>TLC HD</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>13000707</t>
+          <t>13000768</t>
         </is>
       </c>
     </row>
@@ -3812,12 +3812,12 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>TLC HD</t>
+          <t>В мире животных HD</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>13000768</t>
+          <t>13000798</t>
         </is>
       </c>
     </row>
@@ -3829,12 +3829,12 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>В мире животных HD</t>
+          <t>Вопросы и ответы</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>13000798</t>
+          <t>13000801</t>
         </is>
       </c>
     </row>
@@ -3846,12 +3846,12 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>Вопросы и ответы</t>
+          <t>Охота и рыбалка</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>13000801</t>
+          <t>13000766</t>
         </is>
       </c>
     </row>
@@ -3863,12 +3863,12 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>Охота и рыбалка</t>
+          <t>Загородная жизнь HD</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>13000766</t>
+          <t>13000808</t>
         </is>
       </c>
     </row>
@@ -3880,12 +3880,12 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>Загородная жизнь HD</t>
+          <t>Моя Планета HD</t>
         </is>
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>13000808</t>
+          <t>13000767</t>
         </is>
       </c>
     </row>
@@ -3897,12 +3897,12 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>Моя Планета HD</t>
+          <t>Диалоги о рыбалке HD</t>
         </is>
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>13000767</t>
+          <t>13000809</t>
         </is>
       </c>
     </row>
@@ -3914,12 +3914,12 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>Диалоги о рыбалке HD</t>
+          <t>Приключения HD</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>13000809</t>
+          <t>13000558</t>
         </is>
       </c>
     </row>
@@ -3931,12 +3931,12 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>Приключения HD</t>
+          <t>Поехали! HD</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>13000558</t>
+          <t>13000800</t>
         </is>
       </c>
     </row>
@@ -3948,12 +3948,12 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>Поехали! HD</t>
+          <t>Дикая рыбалка HD</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>13000800</t>
+          <t>13000666</t>
         </is>
       </c>
     </row>
@@ -3965,12 +3965,12 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>Дикая рыбалка HD</t>
+          <t>Дикая охота HD</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>13000666</t>
+          <t>13000669</t>
         </is>
       </c>
     </row>
@@ -3982,12 +3982,12 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>Дикая охота HD</t>
+          <t>Оружие</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>13000669</t>
+          <t>13000260</t>
         </is>
       </c>
     </row>
@@ -3999,12 +3999,12 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>Оружие</t>
+          <t>HGTV HD</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>13000260</t>
+          <t>13000203</t>
         </is>
       </c>
     </row>
@@ -4016,12 +4016,12 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>HGTV HD</t>
+          <t>Глазами туриста HD</t>
         </is>
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>13000203</t>
+          <t>13000238</t>
         </is>
       </c>
     </row>
@@ -4033,12 +4033,12 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>Глазами туриста HD</t>
+          <t>Наука 2.0 HD</t>
         </is>
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>13000238</t>
+          <t>13000622</t>
         </is>
       </c>
     </row>
@@ -4050,12 +4050,12 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Наука 2.0 HD</t>
+          <t>DTX HD</t>
         </is>
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>13000622</t>
+          <t>13000194</t>
         </is>
       </c>
     </row>
@@ -4067,12 +4067,12 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>DTX HD</t>
+          <t>Мужской</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>13000194</t>
+          <t>13000802</t>
         </is>
       </c>
     </row>
@@ -4084,12 +4084,12 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Мужской</t>
+          <t>История</t>
         </is>
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>13000802</t>
+          <t>13000815</t>
         </is>
       </c>
     </row>
@@ -4101,12 +4101,12 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>История</t>
+          <t>Кто есть кто</t>
         </is>
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>13000815</t>
+          <t>13000827</t>
         </is>
       </c>
     </row>
@@ -4118,12 +4118,12 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Кто есть кто</t>
+          <t>Travel+Adventure HD</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>13000827</t>
+          <t>13000858</t>
         </is>
       </c>
     </row>
@@ -4135,12 +4135,12 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Travel+Adventure HD</t>
+          <t>365д</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>13000858</t>
+          <t>13000886</t>
         </is>
       </c>
     </row>
@@ -4152,12 +4152,12 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>365 дней HD</t>
+          <t>Звезда Плюс HD</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>13000886</t>
+          <t>13000942</t>
         </is>
       </c>
     </row>
@@ -4169,12 +4169,12 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Звезда Плюс HD</t>
+          <t>24 Техно</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>13000942</t>
+          <t>13000983</t>
         </is>
       </c>
     </row>
@@ -4186,12 +4186,12 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>24 Техно</t>
+          <t>Театр HD</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>13000983</t>
+          <t>13000988</t>
         </is>
       </c>
     </row>
@@ -4203,12 +4203,12 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Театр HD</t>
+          <t>Ностальгия</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>13000988</t>
+          <t>13000786</t>
         </is>
       </c>
     </row>
@@ -4220,12 +4220,12 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>Ностальгия</t>
+          <t>ZooПарк</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>13000786</t>
+          <t>13000989</t>
         </is>
       </c>
     </row>
@@ -4237,12 +4237,12 @@
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>ZooПарк</t>
+          <t>Ретро</t>
         </is>
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>13000989</t>
+          <t>13000785</t>
         </is>
       </c>
     </row>
@@ -4254,12 +4254,12 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Ретро</t>
+          <t>Дикий</t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>13000785</t>
+          <t>13000993</t>
         </is>
       </c>
     </row>
@@ -4271,12 +4271,12 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Дикий</t>
+          <t>Анекдот ТВ</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>13000993</t>
+          <t>13000772</t>
         </is>
       </c>
     </row>
@@ -4288,12 +4288,12 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Анекдот ТВ</t>
+          <t>Рыболов</t>
         </is>
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>13000772</t>
+          <t>13000994</t>
         </is>
       </c>
     </row>
@@ -4305,12 +4305,12 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Рыболов</t>
+          <t>GagsNetwork HD</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>13000994</t>
+          <t>13000825</t>
         </is>
       </c>
     </row>
@@ -4322,12 +4322,12 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Gags Network HD</t>
+          <t>Сарафан</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>13000825</t>
+          <t>13000784</t>
         </is>
       </c>
     </row>
@@ -4339,12 +4339,12 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Сарафан</t>
+          <t>Суббота! HD</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>13000784</t>
+          <t>13000852</t>
         </is>
       </c>
     </row>
@@ -4356,12 +4356,12 @@
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Суббота! HD</t>
+          <t>КВН</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>13000852</t>
+          <t>13000085</t>
         </is>
       </c>
     </row>
@@ -4373,12 +4373,12 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>КВН</t>
+          <t>Бобёр</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>13000085</t>
+          <t>13000235</t>
         </is>
       </c>
     </row>
@@ -4390,12 +4390,12 @@
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Бобёр</t>
+          <t>Тайны галактики HD</t>
         </is>
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>13000235</t>
+          <t>13000683</t>
         </is>
       </c>
     </row>
@@ -4407,12 +4407,12 @@
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Тайны галактики HD</t>
+          <t>Усадьба</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>13000683</t>
+          <t>13000682</t>
         </is>
       </c>
     </row>
@@ -4424,12 +4424,12 @@
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Усадьба</t>
+          <t>2x2</t>
         </is>
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>13000682</t>
+          <t>13000032</t>
         </is>
       </c>
     </row>
@@ -4441,12 +4441,12 @@
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>2x2</t>
+          <t>Cartoonito</t>
         </is>
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>13000032</t>
+          <t>13000720</t>
         </is>
       </c>
     </row>
@@ -4458,12 +4458,12 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Boomerang</t>
+          <t>Cartoon Network</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>13000720</t>
+          <t>13000172</t>
         </is>
       </c>
     </row>
@@ -4475,12 +4475,12 @@
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Cartoon Network</t>
+          <t>Советские мультфильмы</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>13000172</t>
+          <t>13000561</t>
         </is>
       </c>
     </row>
@@ -4492,12 +4492,12 @@
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Советские мультфильмы</t>
+          <t>Gulli Girl</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>13000561</t>
+          <t>13000173</t>
         </is>
       </c>
     </row>
@@ -4509,12 +4509,12 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Gulli Girl</t>
+          <t>Ani</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>13000173</t>
+          <t>13000817</t>
         </is>
       </c>
     </row>
@@ -4526,12 +4526,12 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Ani</t>
+          <t>Nickelodeon HD</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>13000817</t>
+          <t>13000177</t>
         </is>
       </c>
     </row>
@@ -4543,12 +4543,12 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Nickelodeon HD</t>
+          <t>TiJi</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>13000177</t>
+          <t>13001167</t>
         </is>
       </c>
     </row>
@@ -4560,12 +4560,12 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>TiJi</t>
+          <t>Солнце</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>13001167</t>
+          <t>13000037</t>
         </is>
       </c>
     </row>
@@ -4577,12 +4577,12 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Солнце</t>
+          <t>Nick Jr.</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>13000037</t>
+          <t>13000804</t>
         </is>
       </c>
     </row>
@@ -4594,12 +4594,12 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Nick Jr.</t>
+          <t>Кап. Фантастика HD</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>13000804</t>
+          <t>13000614</t>
         </is>
       </c>
     </row>
@@ -4611,12 +4611,12 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Disney RU</t>
+          <t>Nickelodeon</t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>13001172</t>
+          <t>13000805</t>
         </is>
       </c>
     </row>
@@ -4628,12 +4628,12 @@
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Кап. Фантастика HD</t>
+          <t>Мульт HD</t>
         </is>
       </c>
       <c r="C248" t="inlineStr">
         <is>
-          <t>13000614</t>
+          <t>13000181</t>
         </is>
       </c>
     </row>
@@ -4645,12 +4645,12 @@
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Nickelodeon</t>
+          <t>CTC Kids HD</t>
         </is>
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>13000805</t>
+          <t>13000818</t>
         </is>
       </c>
     </row>
@@ -4662,12 +4662,12 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Мульт HD</t>
+          <t>JimJam</t>
         </is>
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>13000181</t>
+          <t>13000859</t>
         </is>
       </c>
     </row>
@@ -4679,12 +4679,12 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>CTC Kids HD</t>
+          <t>О!</t>
         </is>
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>13000818</t>
+          <t>13000187</t>
         </is>
       </c>
     </row>
@@ -4696,12 +4696,12 @@
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>JimJam</t>
+          <t>Мультимузыка</t>
         </is>
       </c>
       <c r="C252" t="inlineStr">
         <is>
-          <t>13000859</t>
+          <t>13000866</t>
         </is>
       </c>
     </row>
@@ -4713,12 +4713,12 @@
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>О!</t>
+          <t>FAN HD</t>
         </is>
       </c>
       <c r="C253" t="inlineStr">
         <is>
-          <t>13000187</t>
+          <t>13000055</t>
         </is>
       </c>
     </row>
@@ -4730,12 +4730,12 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>Мультимузыка</t>
+          <t>Мультиландия</t>
         </is>
       </c>
       <c r="C254" t="inlineStr">
         <is>
-          <t>13000866</t>
+          <t>13000867</t>
         </is>
       </c>
     </row>
@@ -4747,12 +4747,12 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>FAN HD</t>
+          <t>Рыжий</t>
         </is>
       </c>
       <c r="C255" t="inlineStr">
         <is>
-          <t>13000055</t>
+          <t>13000578</t>
         </is>
       </c>
     </row>
@@ -4764,12 +4764,12 @@
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>Мультиландия</t>
+          <t>Радость моя</t>
         </is>
       </c>
       <c r="C256" t="inlineStr">
         <is>
-          <t>13000867</t>
+          <t>13000696</t>
         </is>
       </c>
     </row>
@@ -4781,12 +4781,12 @@
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>Рыжий</t>
+          <t>Уникум!</t>
         </is>
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>13000578</t>
+          <t>13000865</t>
         </is>
       </c>
     </row>
@@ -4798,12 +4798,12 @@
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>Радость моя</t>
+          <t>ПЕРВЫЙ +1</t>
         </is>
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>13000696</t>
+          <t>13000876</t>
         </is>
       </c>
     </row>
@@ -4815,12 +4815,12 @@
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>Baby TV</t>
+          <t>ПЕРВЫЙ +2</t>
         </is>
       </c>
       <c r="C259" t="inlineStr">
         <is>
-          <t>13000941</t>
+          <t>13000831</t>
         </is>
       </c>
     </row>
@@ -4832,12 +4832,12 @@
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>Уникум!</t>
+          <t>ПЕРВЫЙ +3</t>
         </is>
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>13000865</t>
+          <t>13000877</t>
         </is>
       </c>
     </row>
@@ -4849,12 +4849,12 @@
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>ПЕРВЫЙ +1</t>
+          <t>ПЕРВЫЙ +4</t>
         </is>
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>13000876</t>
+          <t>13000484</t>
         </is>
       </c>
     </row>
@@ -4866,12 +4866,12 @@
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>ПЕРВЫЙ +2</t>
+          <t>ПЕРВЫЙ +5</t>
         </is>
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>13000831</t>
+          <t>13000878</t>
         </is>
       </c>
     </row>
@@ -4883,12 +4883,12 @@
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>ПЕРВЫЙ +3</t>
+          <t>ПЕРВЫЙ +7</t>
         </is>
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>13000877</t>
+          <t>13000832</t>
         </is>
       </c>
     </row>
@@ -4900,12 +4900,12 @@
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>ПЕРВЫЙ +4</t>
+          <t>ПЕРВЫЙ +8</t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>13000484</t>
+          <t>13000879</t>
         </is>
       </c>
     </row>
@@ -4917,12 +4917,12 @@
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>ПЕРВЫЙ +5</t>
+          <t>РОССИЯ-1 +1</t>
         </is>
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>13000878</t>
+          <t>13000010</t>
         </is>
       </c>
     </row>
@@ -4934,12 +4934,12 @@
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>ПЕРВЫЙ +7</t>
+          <t>РОССИЯ-1 +2</t>
         </is>
       </c>
       <c r="C266" t="inlineStr">
         <is>
-          <t>13000832</t>
+          <t>13000493</t>
         </is>
       </c>
     </row>
@@ -4951,12 +4951,12 @@
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>ПЕРВЫЙ +8</t>
+          <t>РОССИЯ-1 +4</t>
         </is>
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>13000879</t>
+          <t>13000494</t>
         </is>
       </c>
     </row>
@@ -4968,12 +4968,12 @@
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>РОССИЯ-1 +1</t>
+          <t>РОССИЯ-1 +9</t>
         </is>
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>13000010</t>
+          <t>13000495</t>
         </is>
       </c>
     </row>
@@ -4985,12 +4985,12 @@
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>РОССИЯ-1 +2</t>
+          <t>НТВ +2</t>
         </is>
       </c>
       <c r="C269" t="inlineStr">
         <is>
-          <t>13000493</t>
+          <t>13000829</t>
         </is>
       </c>
     </row>
@@ -5002,12 +5002,12 @@
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>РОССИЯ-1 +4</t>
+          <t>НТВ +7</t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>13000494</t>
+          <t>13000830</t>
         </is>
       </c>
     </row>
@@ -5019,12 +5019,12 @@
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>РОССИЯ-1 +9</t>
+          <t>ТНТ +2</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>13000495</t>
+          <t>13000861</t>
         </is>
       </c>
     </row>
@@ -5036,12 +5036,12 @@
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>НТВ +2</t>
+          <t>ТНТ +4</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>13000829</t>
+          <t>13000882</t>
         </is>
       </c>
     </row>
@@ -5053,12 +5053,12 @@
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>НТВ +7</t>
+          <t>ТНТ +7</t>
         </is>
       </c>
       <c r="C273" t="inlineStr">
         <is>
-          <t>13000830</t>
+          <t>13000883</t>
         </is>
       </c>
     </row>
@@ -5070,12 +5070,12 @@
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>ТНТ +2</t>
+          <t>СТС +4</t>
         </is>
       </c>
       <c r="C274" t="inlineStr">
         <is>
-          <t>13000861</t>
+          <t>13000880</t>
         </is>
       </c>
     </row>
@@ -5087,12 +5087,12 @@
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>ТНТ +4</t>
+          <t>Пятница! +4</t>
         </is>
       </c>
       <c r="C275" t="inlineStr">
         <is>
-          <t>13000882</t>
+          <t>13000884</t>
         </is>
       </c>
     </row>
@@ -5104,12 +5104,12 @@
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>ТНТ +7</t>
+          <t>Пятница! +6</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>13000883</t>
+          <t>13000885</t>
         </is>
       </c>
     </row>
@@ -5121,12 +5121,12 @@
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>СТС +4</t>
+          <t>RU.TV HD</t>
         </is>
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>13000880</t>
+          <t>13000154</t>
         </is>
       </c>
     </row>
@@ -5138,12 +5138,12 @@
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Пятница! +4</t>
+          <t>1HD Music Television</t>
         </is>
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>13000884</t>
+          <t>13000675</t>
         </is>
       </c>
     </row>
@@ -5155,12 +5155,12 @@
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Пятница! +6</t>
+          <t>Europa Plus TV HD</t>
         </is>
       </c>
       <c r="C279" t="inlineStr">
         <is>
-          <t>13000885</t>
+          <t>13000812</t>
         </is>
       </c>
     </row>
@@ -5172,12 +5172,12 @@
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>RU.TV HD</t>
+          <t>Bridge Classic</t>
         </is>
       </c>
       <c r="C280" t="inlineStr">
         <is>
-          <t>13000154</t>
+          <t>13000141</t>
         </is>
       </c>
     </row>
@@ -5189,12 +5189,12 @@
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>1HD Music Television</t>
+          <t>Russian MusicBox HD</t>
         </is>
       </c>
       <c r="C281" t="inlineStr">
         <is>
-          <t>13000675</t>
+          <t>13000813</t>
         </is>
       </c>
     </row>
@@ -5206,12 +5206,12 @@
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Europa Plus TV HD</t>
+          <t>VB Dance Hits of 90s</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>13000812</t>
+          <t>13001181</t>
         </is>
       </c>
     </row>
@@ -5223,12 +5223,12 @@
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Bridge Classic</t>
+          <t>Bridge Hits</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>13000141</t>
+          <t>13000143</t>
         </is>
       </c>
     </row>
@@ -5240,12 +5240,12 @@
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Russian MusicBox HD</t>
+          <t>VB Eurodance Hits 90s</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>13000813</t>
+          <t>13001182</t>
         </is>
       </c>
     </row>
@@ -5257,12 +5257,12 @@
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>VB Dance Hits of 90s</t>
+          <t>Bridge Русский Хит</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
         <is>
-          <t>13001181</t>
+          <t>13000144</t>
         </is>
       </c>
     </row>
@@ -5274,12 +5274,12 @@
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Bridge Hits</t>
+          <t>VB Русская попса 80х-90х</t>
         </is>
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>13000143</t>
+          <t>13001187</t>
         </is>
       </c>
     </row>
@@ -5291,12 +5291,12 @@
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>VB Eurodance Hits 90s</t>
+          <t>Bridge Deluxe HD</t>
         </is>
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>13001182</t>
+          <t>13000142</t>
         </is>
       </c>
     </row>
@@ -5308,12 +5308,12 @@
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Bridge Русский Хит</t>
+          <t>4ever Music HD</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
         <is>
-          <t>13000144</t>
+          <t>13000833</t>
         </is>
       </c>
     </row>
@@ -5325,12 +5325,12 @@
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>VB Русская попса 80х-90х</t>
+          <t>VB Best Live Performances</t>
         </is>
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>13001187</t>
+          <t>13001190</t>
         </is>
       </c>
     </row>
@@ -5342,12 +5342,12 @@
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Bridge Deluxe HD</t>
+          <t>Bridge</t>
         </is>
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>13000142</t>
+          <t>13000140</t>
         </is>
       </c>
     </row>
@@ -5359,12 +5359,12 @@
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>4ever Music HD</t>
+          <t>Bridge Rock</t>
         </is>
       </c>
       <c r="C291" t="inlineStr">
         <is>
-          <t>13000833</t>
+          <t>13001008</t>
         </is>
       </c>
     </row>
@@ -5376,12 +5376,12 @@
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>VB Best Live Performances</t>
+          <t>VB MTV OLD</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>13001190</t>
+          <t>13001193</t>
         </is>
       </c>
     </row>
@@ -5393,12 +5393,12 @@
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Bridge</t>
+          <t>Bridge Шлягер</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>13000140</t>
+          <t>13000619</t>
         </is>
       </c>
     </row>
@@ -5410,12 +5410,12 @@
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>Bridge Rock</t>
+          <t>VB Russian Dance Hits of 90</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>13001008</t>
+          <t>13001194</t>
         </is>
       </c>
     </row>
@@ -5427,12 +5427,12 @@
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>VB MTV OLD</t>
+          <t>VB Greatest Hits</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>13001193</t>
+          <t>13001195</t>
         </is>
       </c>
     </row>
@@ -5444,12 +5444,12 @@
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>Bridge Шлягер</t>
+          <t>VB Romantic and Ballads</t>
         </is>
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>13000619</t>
+          <t>13001196</t>
         </is>
       </c>
     </row>
@@ -5461,12 +5461,12 @@
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>VB Russian Dance Hits of 90</t>
+          <t>Музыка Первого</t>
         </is>
       </c>
       <c r="C297" t="inlineStr">
         <is>
-          <t>13001194</t>
+          <t>13000790</t>
         </is>
       </c>
     </row>
@@ -5478,12 +5478,12 @@
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>VB Greatest Hits</t>
+          <t>РОК НАРЯД HD</t>
         </is>
       </c>
       <c r="C298" t="inlineStr">
         <is>
-          <t>13001195</t>
+          <t>13000658</t>
         </is>
       </c>
     </row>
@@ -5495,12 +5495,12 @@
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>VB Romantic and Ballads</t>
+          <t>MCM-TOP</t>
         </is>
       </c>
       <c r="C299" t="inlineStr">
         <is>
-          <t>13001196</t>
+          <t>13000803</t>
         </is>
       </c>
     </row>
@@ -5512,12 +5512,12 @@
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>Музыка Первого</t>
+          <t>MTV 80's</t>
         </is>
       </c>
       <c r="C300" t="inlineStr">
         <is>
-          <t>13000790</t>
+          <t>13000158</t>
         </is>
       </c>
     </row>
@@ -5529,12 +5529,12 @@
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>РОК НАРЯД HD</t>
+          <t>О!2</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
         <is>
-          <t>13000658</t>
+          <t>13000814</t>
         </is>
       </c>
     </row>
@@ -5546,12 +5546,12 @@
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>MCM-TOP</t>
+          <t>MTV 90's</t>
         </is>
       </c>
       <c r="C302" t="inlineStr">
         <is>
-          <t>13000803</t>
+          <t>13000151</t>
         </is>
       </c>
     </row>
@@ -5563,12 +5563,12 @@
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>MTV 80's</t>
+          <t>MTV Club</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
         <is>
-          <t>13000158</t>
+          <t>13000147</t>
         </is>
       </c>
     </row>
@@ -5580,12 +5580,12 @@
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>О!2</t>
+          <t>Clubbing TV HD</t>
         </is>
       </c>
       <c r="C304" t="inlineStr">
         <is>
-          <t>13000814</t>
+          <t>13000837</t>
         </is>
       </c>
     </row>
@@ -5597,12 +5597,12 @@
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>MTV 90's</t>
+          <t>MTV Hits</t>
         </is>
       </c>
       <c r="C305" t="inlineStr">
         <is>
-          <t>13000151</t>
+          <t>13000149</t>
         </is>
       </c>
     </row>
@@ -5614,12 +5614,12 @@
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>MTV Club</t>
+          <t>Жара HD</t>
         </is>
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>13000147</t>
+          <t>13000860</t>
         </is>
       </c>
     </row>
@@ -5631,12 +5631,12 @@
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>Clubbing TV HD</t>
+          <t>iConcerts HD</t>
         </is>
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>13000837</t>
+          <t>13000944</t>
         </is>
       </c>
     </row>
@@ -5648,12 +5648,12 @@
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>MTV Hits</t>
+          <t>Stingray CMusic HD</t>
         </is>
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>13000149</t>
+          <t>13000945</t>
         </is>
       </c>
     </row>
@@ -5665,12 +5665,12 @@
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>Жара HD</t>
+          <t>MTV 00's</t>
         </is>
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>13000860</t>
+          <t>13000159</t>
         </is>
       </c>
     </row>
@@ -5682,12 +5682,12 @@
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>iConcerts HD</t>
+          <t>ТНТ Music HD</t>
         </is>
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>13000944</t>
+          <t>13000685</t>
         </is>
       </c>
     </row>
@@ -5699,12 +5699,12 @@
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>Stingray CMusic HD</t>
+          <t>Шансон-ТВ</t>
         </is>
       </c>
       <c r="C311" t="inlineStr">
         <is>
-          <t>13000945</t>
+          <t>13000679</t>
         </is>
       </c>
     </row>
@@ -5716,12 +5716,12 @@
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>MTV 00's</t>
+          <t>Жар Птица</t>
         </is>
       </c>
       <c r="C312" t="inlineStr">
         <is>
-          <t>13000159</t>
+          <t>13000928</t>
         </is>
       </c>
     </row>
@@ -5733,12 +5733,12 @@
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>ТНТ Music HD</t>
+          <t>Karloson TV Том и Джерри HD</t>
         </is>
       </c>
       <c r="C313" t="inlineStr">
         <is>
-          <t>13000685</t>
+          <t>13000977</t>
         </is>
       </c>
     </row>
@@ -5750,12 +5750,12 @@
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>Шансон-ТВ</t>
+          <t>Karloson TV Чёрный плащ HD</t>
         </is>
       </c>
       <c r="C314" t="inlineStr">
         <is>
-          <t>13000679</t>
+          <t>13000982</t>
         </is>
       </c>
     </row>
@@ -5767,12 +5767,12 @@
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>Жар Птица</t>
+          <t>VIP Comedy HD CEE</t>
         </is>
       </c>
       <c r="C315" t="inlineStr">
         <is>
-          <t>13000928</t>
+          <t>13001030</t>
         </is>
       </c>
     </row>
@@ -5784,12 +5784,12 @@
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>Karloson TV Том и Джерри HD</t>
+          <t>VIP Megahit HD CEE</t>
         </is>
       </c>
       <c r="C316" t="inlineStr">
         <is>
-          <t>13000977</t>
+          <t>13001031</t>
         </is>
       </c>
     </row>
@@ -5801,12 +5801,12 @@
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>Karloson TV Чёрный плащ HD</t>
+          <t>Тайна</t>
         </is>
       </c>
       <c r="C317" t="inlineStr">
         <is>
-          <t>13000982</t>
+          <t>13001033</t>
         </is>
       </c>
     </row>
@@ -5818,12 +5818,12 @@
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>VIP Comedy HD CEE</t>
+          <t>C-Cartoon HD</t>
         </is>
       </c>
       <c r="C318" t="inlineStr">
         <is>
-          <t>13001030</t>
+          <t>13001035</t>
         </is>
       </c>
     </row>
@@ -5835,12 +5835,12 @@
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>VIP Megahit HD CEE</t>
+          <t>C-Inquest HD</t>
         </is>
       </c>
       <c r="C319" t="inlineStr">
         <is>
-          <t>13001031</t>
+          <t>13001036</t>
         </is>
       </c>
     </row>
@@ -5852,12 +5852,12 @@
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>VIP Premiere HD CEE</t>
+          <t>C-Comedy HD</t>
         </is>
       </c>
       <c r="C320" t="inlineStr">
         <is>
-          <t>13001032</t>
+          <t>13001037</t>
         </is>
       </c>
     </row>
@@ -5869,12 +5869,12 @@
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>Тайна</t>
+          <t>YOSSO TV MUSIC HITS HD</t>
         </is>
       </c>
       <c r="C321" t="inlineStr">
         <is>
-          <t>13001033</t>
+          <t>13001038</t>
         </is>
       </c>
     </row>
@@ -5886,12 +5886,12 @@
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>C-Cartoon HD</t>
+          <t>YOSSO TV OBLIVION HD</t>
         </is>
       </c>
       <c r="C322" t="inlineStr">
         <is>
-          <t>13001035</t>
+          <t>13001039</t>
         </is>
       </c>
     </row>
@@ -5903,12 +5903,12 @@
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>C-Inquest HD</t>
+          <t>Рен ТВ (+4)</t>
         </is>
       </c>
       <c r="C323" t="inlineStr">
         <is>
-          <t>13001036</t>
+          <t>13001041</t>
         </is>
       </c>
     </row>
@@ -5920,12 +5920,12 @@
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>C-Comedy HD</t>
+          <t>Рен ТВ (+7)</t>
         </is>
       </c>
       <c r="C324" t="inlineStr">
         <is>
-          <t>13001037</t>
+          <t>13001042</t>
         </is>
       </c>
     </row>
@@ -5937,12 +5937,12 @@
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>YOSSO TV MUSIC HITS HD</t>
+          <t>TV1000 World Kino</t>
         </is>
       </c>
       <c r="C325" t="inlineStr">
         <is>
-          <t>13001038</t>
+          <t>13001043</t>
         </is>
       </c>
     </row>
@@ -5954,12 +5954,12 @@
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>YOSSO TV OBLIVION HD</t>
+          <t>TV1000 CEE HD</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
         <is>
-          <t>13001039</t>
+          <t>13001044</t>
         </is>
       </c>
     </row>
@@ -5971,12 +5971,12 @@
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>Рен ТВ (+4)</t>
+          <t>TV1000 Action CEE HD</t>
         </is>
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>13001041</t>
+          <t>13001045</t>
         </is>
       </c>
     </row>
@@ -5988,12 +5988,12 @@
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>Рен ТВ (+7)</t>
+          <t>Футбольный HD</t>
         </is>
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>13001042</t>
+          <t>13001046</t>
         </is>
       </c>
     </row>
@@ -6005,12 +6005,12 @@
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>TV1000 World Kino</t>
+          <t>Хоккейный HD</t>
         </is>
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>13001043</t>
+          <t>13001047</t>
         </is>
       </c>
     </row>
@@ -6022,12 +6022,12 @@
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>TV1000 CEE HD</t>
+          <t>Спортивный HD</t>
         </is>
       </c>
       <c r="C330" t="inlineStr">
         <is>
-          <t>13001044</t>
+          <t>13001048</t>
         </is>
       </c>
     </row>
@@ -6039,12 +6039,12 @@
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>TV1000 Action CEE HD</t>
+          <t>Синема HD</t>
         </is>
       </c>
       <c r="C331" t="inlineStr">
         <is>
-          <t>13001045</t>
+          <t>13001049</t>
         </is>
       </c>
     </row>
@@ -6056,12 +6056,12 @@
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>Футбольный HD</t>
+          <t>Kernel TV Леди Баг HD</t>
         </is>
       </c>
       <c r="C332" t="inlineStr">
         <is>
-          <t>13001046</t>
+          <t>13001052</t>
         </is>
       </c>
     </row>
@@ -6073,12 +6073,12 @@
       </c>
       <c r="B333" t="inlineStr">
         <is>
-          <t>Хоккейный HD</t>
+          <t>Kernel TV Маша и Медведь HD</t>
         </is>
       </c>
       <c r="C333" t="inlineStr">
         <is>
-          <t>13001047</t>
+          <t>13001053</t>
         </is>
       </c>
     </row>
@@ -6090,12 +6090,12 @@
       </c>
       <c r="B334" t="inlineStr">
         <is>
-          <t>Спортивный HD</t>
+          <t>Kernel TV Драконы и всадники Олуха HD</t>
         </is>
       </c>
       <c r="C334" t="inlineStr">
         <is>
-          <t>13001048</t>
+          <t>13001054</t>
         </is>
       </c>
     </row>
@@ -6107,12 +6107,12 @@
       </c>
       <c r="B335" t="inlineStr">
         <is>
-          <t>Синема HD</t>
+          <t>Kernel TV Царевны HD</t>
         </is>
       </c>
       <c r="C335" t="inlineStr">
         <is>
-          <t>13001049</t>
+          <t>13001055</t>
         </is>
       </c>
     </row>
@@ -6124,12 +6124,12 @@
       </c>
       <c r="B336" t="inlineStr">
         <is>
-          <t>Kernel TV Леди Баг HD</t>
+          <t>Kernel TV Человек-паук 2012 HD</t>
         </is>
       </c>
       <c r="C336" t="inlineStr">
         <is>
-          <t>13001052</t>
+          <t>13001056</t>
         </is>
       </c>
     </row>
@@ -6141,12 +6141,12 @@
       </c>
       <c r="B337" t="inlineStr">
         <is>
-          <t>Kernel TV Маша и Медведь HD</t>
+          <t>ПЕРВЫЙ +6</t>
         </is>
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>13001053</t>
+          <t>13001057</t>
         </is>
       </c>
     </row>
@@ -6158,12 +6158,12 @@
       </c>
       <c r="B338" t="inlineStr">
         <is>
-          <t>Kernel TV Драконы и всадники Олуха HD</t>
+          <t>Kernel TV Финес и Ферб HD</t>
         </is>
       </c>
       <c r="C338" t="inlineStr">
         <is>
-          <t>13001054</t>
+          <t>13001058</t>
         </is>
       </c>
     </row>
@@ -6175,12 +6175,12 @@
       </c>
       <c r="B339" t="inlineStr">
         <is>
-          <t>Kernel TV Царевны HD</t>
+          <t>Kernel TV Люк - путешественник во времени HD</t>
         </is>
       </c>
       <c r="C339" t="inlineStr">
         <is>
-          <t>13001055</t>
+          <t>13001059</t>
         </is>
       </c>
     </row>
@@ -6192,12 +6192,12 @@
       </c>
       <c r="B340" t="inlineStr">
         <is>
-          <t>Kernel TV Человек-паук 2012 HD</t>
+          <t>Kernel TV Смешарики HD</t>
         </is>
       </c>
       <c r="C340" t="inlineStr">
         <is>
-          <t>13001056</t>
+          <t>13001060</t>
         </is>
       </c>
     </row>
@@ -6209,12 +6209,12 @@
       </c>
       <c r="B341" t="inlineStr">
         <is>
-          <t>ПЕРВЫЙ +6</t>
+          <t>Kernel TV Команда Турбо HD</t>
         </is>
       </c>
       <c r="C341" t="inlineStr">
         <is>
-          <t>13001057</t>
+          <t>13001061</t>
         </is>
       </c>
     </row>
@@ -6226,12 +6226,12 @@
       </c>
       <c r="B342" t="inlineStr">
         <is>
-          <t>Kernel TV Финес и Ферб HD</t>
+          <t>Kernel TV Гравити Фолз HD</t>
         </is>
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>13001058</t>
+          <t>13001063</t>
         </is>
       </c>
     </row>
@@ -6243,12 +6243,12 @@
       </c>
       <c r="B343" t="inlineStr">
         <is>
-          <t>Kernel TV Люк - путешественник во времени HD</t>
+          <t>Kernel TV Фиксики HD</t>
         </is>
       </c>
       <c r="C343" t="inlineStr">
         <is>
-          <t>13001059</t>
+          <t>13001064</t>
         </is>
       </c>
     </row>
@@ -6260,12 +6260,12 @@
       </c>
       <c r="B344" t="inlineStr">
         <is>
-          <t>Kernel TV Смешарики HD</t>
+          <t>Kernel TV Лило и Стич HD</t>
         </is>
       </c>
       <c r="C344" t="inlineStr">
         <is>
-          <t>13001060</t>
+          <t>13001065</t>
         </is>
       </c>
     </row>
@@ -6277,12 +6277,12 @@
       </c>
       <c r="B345" t="inlineStr">
         <is>
-          <t>Kernel TV Команда Турбо HD</t>
+          <t>Kernel TV Том и Джерри HD</t>
         </is>
       </c>
       <c r="C345" t="inlineStr">
         <is>
-          <t>13001061</t>
+          <t>13001066</t>
         </is>
       </c>
     </row>
@@ -6294,12 +6294,12 @@
       </c>
       <c r="B346" t="inlineStr">
         <is>
-          <t>Kernel TV Гравити Фолз HD</t>
+          <t>Kernel TV Три кота HD</t>
         </is>
       </c>
       <c r="C346" t="inlineStr">
         <is>
-          <t>13001063</t>
+          <t>13001067</t>
         </is>
       </c>
     </row>
@@ -6311,12 +6311,12 @@
       </c>
       <c r="B347" t="inlineStr">
         <is>
-          <t>Kernel TV Фиксики HD</t>
+          <t>Kernel TV Футурама HD</t>
         </is>
       </c>
       <c r="C347" t="inlineStr">
         <is>
-          <t>13001064</t>
+          <t>13001070</t>
         </is>
       </c>
     </row>
@@ -6328,12 +6328,12 @@
       </c>
       <c r="B348" t="inlineStr">
         <is>
-          <t>Kernel TV Лило и Стич HD</t>
+          <t>Тип-Топ HD</t>
         </is>
       </c>
       <c r="C348" t="inlineStr">
         <is>
-          <t>13001065</t>
+          <t>13001071</t>
         </is>
       </c>
     </row>
@@ -6345,12 +6345,12 @@
       </c>
       <c r="B349" t="inlineStr">
         <is>
-          <t>Kernel TV Том и Джерри HD</t>
+          <t>Ю (+2)</t>
         </is>
       </c>
       <c r="C349" t="inlineStr">
         <is>
-          <t>13001066</t>
+          <t>13001073</t>
         </is>
       </c>
     </row>
@@ -6362,12 +6362,12 @@
       </c>
       <c r="B350" t="inlineStr">
         <is>
-          <t>Kernel TV Три кота HD</t>
+          <t>Ю (+4)</t>
         </is>
       </c>
       <c r="C350" t="inlineStr">
         <is>
-          <t>13001067</t>
+          <t>13001074</t>
         </is>
       </c>
     </row>
@@ -6379,12 +6379,12 @@
       </c>
       <c r="B351" t="inlineStr">
         <is>
-          <t>Kernel TV Футурама HD</t>
+          <t>Ю (+7)</t>
         </is>
       </c>
       <c r="C351" t="inlineStr">
         <is>
-          <t>13001070</t>
+          <t>13001075</t>
         </is>
       </c>
     </row>
@@ -6396,12 +6396,12 @@
       </c>
       <c r="B352" t="inlineStr">
         <is>
-          <t>Тип-Топ HD</t>
+          <t>Первый канал HD (+4)</t>
         </is>
       </c>
       <c r="C352" t="inlineStr">
         <is>
-          <t>13001071</t>
+          <t>13001076</t>
         </is>
       </c>
     </row>
@@ -6413,12 +6413,12 @@
       </c>
       <c r="B353" t="inlineStr">
         <is>
-          <t>Ю (+2)</t>
+          <t>Сваты 24/7</t>
         </is>
       </c>
       <c r="C353" t="inlineStr">
         <is>
-          <t>13001073</t>
+          <t>13001077</t>
         </is>
       </c>
     </row>
@@ -6430,12 +6430,12 @@
       </c>
       <c r="B354" t="inlineStr">
         <is>
-          <t>Ю (+4)</t>
+          <t>НТВ Хит</t>
         </is>
       </c>
       <c r="C354" t="inlineStr">
         <is>
-          <t>13001074</t>
+          <t>13001078</t>
         </is>
       </c>
     </row>
@@ -6447,12 +6447,12 @@
       </c>
       <c r="B355" t="inlineStr">
         <is>
-          <t>Ю (+7)</t>
+          <t>НТВ Стиль</t>
         </is>
       </c>
       <c r="C355" t="inlineStr">
         <is>
-          <t>13001075</t>
+          <t>13001079</t>
         </is>
       </c>
     </row>
@@ -6464,12 +6464,12 @@
       </c>
       <c r="B356" t="inlineStr">
         <is>
-          <t>Первый канал HD (+4)</t>
+          <t>НТВ Сериал</t>
         </is>
       </c>
       <c r="C356" t="inlineStr">
         <is>
-          <t>13001076</t>
+          <t>13001080</t>
         </is>
       </c>
     </row>
@@ -6481,12 +6481,12 @@
       </c>
       <c r="B357" t="inlineStr">
         <is>
-          <t>Сваты 24/7</t>
+          <t>НТВ Право</t>
         </is>
       </c>
       <c r="C357" t="inlineStr">
         <is>
-          <t>13001077</t>
+          <t>13001081</t>
         </is>
       </c>
     </row>
@@ -6498,12 +6498,12 @@
       </c>
       <c r="B358" t="inlineStr">
         <is>
-          <t>НТВ Хит</t>
+          <t>Мир баскетбола</t>
         </is>
       </c>
       <c r="C358" t="inlineStr">
         <is>
-          <t>13001078</t>
+          <t>13001084</t>
         </is>
       </c>
     </row>
@@ -6515,12 +6515,12 @@
       </c>
       <c r="B359" t="inlineStr">
         <is>
-          <t>НТВ Стиль</t>
+          <t>Еврокино</t>
         </is>
       </c>
       <c r="C359" t="inlineStr">
         <is>
-          <t>13001079</t>
+          <t>13001085</t>
         </is>
       </c>
     </row>
@@ -6532,12 +6532,12 @@
       </c>
       <c r="B360" t="inlineStr">
         <is>
-          <t>НТВ Сериал</t>
+          <t>Старт HD</t>
         </is>
       </c>
       <c r="C360" t="inlineStr">
         <is>
-          <t>13001080</t>
+          <t>13001086</t>
         </is>
       </c>
     </row>
@@ -6549,12 +6549,12 @@
       </c>
       <c r="B361" t="inlineStr">
         <is>
-          <t>НТВ Право</t>
+          <t>Viasat Explore CEE HD</t>
         </is>
       </c>
       <c r="C361" t="inlineStr">
         <is>
-          <t>13001081</t>
+          <t>13001087</t>
         </is>
       </c>
     </row>
@@ -6566,12 +6566,12 @@
       </c>
       <c r="B362" t="inlineStr">
         <is>
-          <t>Filmzone HD</t>
+          <t>Food Network HD</t>
         </is>
       </c>
       <c r="C362" t="inlineStr">
         <is>
-          <t>13001082</t>
+          <t>13001090</t>
         </is>
       </c>
     </row>
@@ -6583,12 +6583,12 @@
       </c>
       <c r="B363" t="inlineStr">
         <is>
-          <t>Filmzone+ HD</t>
+          <t>Доктор</t>
         </is>
       </c>
       <c r="C363" t="inlineStr">
         <is>
-          <t>13001083</t>
+          <t>13001091</t>
         </is>
       </c>
     </row>
@@ -6600,12 +6600,12 @@
       </c>
       <c r="B364" t="inlineStr">
         <is>
-          <t>Мир баскетбола</t>
+          <t>Индия</t>
         </is>
       </c>
       <c r="C364" t="inlineStr">
         <is>
-          <t>13001084</t>
+          <t>13001092</t>
         </is>
       </c>
     </row>
@@ -6617,12 +6617,12 @@
       </c>
       <c r="B365" t="inlineStr">
         <is>
-          <t>Еврокино</t>
+          <t>NHL Network HD</t>
         </is>
       </c>
       <c r="C365" t="inlineStr">
         <is>
-          <t>13001085</t>
+          <t>13001093</t>
         </is>
       </c>
     </row>
@@ -6634,12 +6634,12 @@
       </c>
       <c r="B366" t="inlineStr">
         <is>
-          <t>Старт HD</t>
+          <t>Домашний Int.</t>
         </is>
       </c>
       <c r="C366" t="inlineStr">
         <is>
-          <t>13001086</t>
+          <t>13001094</t>
         </is>
       </c>
     </row>
@@ -6651,12 +6651,12 @@
       </c>
       <c r="B367" t="inlineStr">
         <is>
-          <t>Viasat Explore CEE HD</t>
+          <t>СуперГерои</t>
         </is>
       </c>
       <c r="C367" t="inlineStr">
         <is>
-          <t>13001087</t>
+          <t>13001095</t>
         </is>
       </c>
     </row>
@@ -6668,12 +6668,12 @@
       </c>
       <c r="B368" t="inlineStr">
         <is>
-          <t>Food Network HD</t>
+          <t>Fast Fun Box HD</t>
         </is>
       </c>
       <c r="C368" t="inlineStr">
         <is>
-          <t>13001090</t>
+          <t>13001096</t>
         </is>
       </c>
     </row>
@@ -6685,12 +6685,12 @@
       </c>
       <c r="B369" t="inlineStr">
         <is>
-          <t>Доктор</t>
+          <t>Индийское кино</t>
         </is>
       </c>
       <c r="C369" t="inlineStr">
         <is>
-          <t>13001091</t>
+          <t>13001097</t>
         </is>
       </c>
     </row>
@@ -6702,12 +6702,12 @@
       </c>
       <c r="B370" t="inlineStr">
         <is>
-          <t>Индия</t>
+          <t>Наше HD</t>
         </is>
       </c>
       <c r="C370" t="inlineStr">
         <is>
-          <t>13001092</t>
+          <t>13001098</t>
         </is>
       </c>
     </row>
@@ -6719,12 +6719,12 @@
       </c>
       <c r="B371" t="inlineStr">
         <is>
-          <t>NHL Network HD</t>
+          <t>Живая природа HD</t>
         </is>
       </c>
       <c r="C371" t="inlineStr">
         <is>
-          <t>13001093</t>
+          <t>13001100</t>
         </is>
       </c>
     </row>
@@ -6736,12 +6736,12 @@
       </c>
       <c r="B372" t="inlineStr">
         <is>
-          <t>Домашний Int.</t>
+          <t>Лёва HD</t>
         </is>
       </c>
       <c r="C372" t="inlineStr">
         <is>
-          <t>13001094</t>
+          <t>13001101</t>
         </is>
       </c>
     </row>
@@ -6753,12 +6753,12 @@
       </c>
       <c r="B373" t="inlineStr">
         <is>
-          <t>СуперГерои</t>
+          <t>Song TV Russia HD</t>
         </is>
       </c>
       <c r="C373" t="inlineStr">
         <is>
-          <t>13001095</t>
+          <t>13001102</t>
         </is>
       </c>
     </row>
@@ -6770,12 +6770,12 @@
       </c>
       <c r="B374" t="inlineStr">
         <is>
-          <t>Fast Fun Box HD</t>
+          <t>Пингвин</t>
         </is>
       </c>
       <c r="C374" t="inlineStr">
         <is>
-          <t>13001096</t>
+          <t>13001104</t>
         </is>
       </c>
     </row>
@@ -6787,12 +6787,12 @@
       </c>
       <c r="B375" t="inlineStr">
         <is>
-          <t>Индийское кино</t>
+          <t>Еда</t>
         </is>
       </c>
       <c r="C375" t="inlineStr">
         <is>
-          <t>13001097</t>
+          <t>13001105</t>
         </is>
       </c>
     </row>
@@ -6804,12 +6804,12 @@
       </c>
       <c r="B376" t="inlineStr">
         <is>
-          <t>Наше HD</t>
+          <t>Родное кино</t>
         </is>
       </c>
       <c r="C376" t="inlineStr">
         <is>
-          <t>13001098</t>
+          <t>13001106</t>
         </is>
       </c>
     </row>
@@ -6821,12 +6821,12 @@
       </c>
       <c r="B377" t="inlineStr">
         <is>
-          <t>BBC World News HD</t>
+          <t>К-Хит HD</t>
         </is>
       </c>
       <c r="C377" t="inlineStr">
         <is>
-          <t>13001099</t>
+          <t>13001107</t>
         </is>
       </c>
     </row>
@@ -6838,12 +6838,12 @@
       </c>
       <c r="B378" t="inlineStr">
         <is>
-          <t>Живая природа HD</t>
+          <t>Зоо ТВ</t>
         </is>
       </c>
       <c r="C378" t="inlineStr">
         <is>
-          <t>13001100</t>
+          <t>13001108</t>
         </is>
       </c>
     </row>
@@ -6855,12 +6855,12 @@
       </c>
       <c r="B379" t="inlineStr">
         <is>
-          <t>Лёва HD</t>
+          <t>Живи Активно HD</t>
         </is>
       </c>
       <c r="C379" t="inlineStr">
         <is>
-          <t>13001101</t>
+          <t>13001110</t>
         </is>
       </c>
     </row>
@@ -6872,12 +6872,12 @@
       </c>
       <c r="B380" t="inlineStr">
         <is>
-          <t>Song TV Russia HD</t>
+          <t>Живи! HD</t>
         </is>
       </c>
       <c r="C380" t="inlineStr">
         <is>
-          <t>13001102</t>
+          <t>13001111</t>
         </is>
       </c>
     </row>
@@ -6889,12 +6889,12 @@
       </c>
       <c r="B381" t="inlineStr">
         <is>
-          <t>Disney Junior</t>
+          <t>Карусель HD</t>
         </is>
       </c>
       <c r="C381" t="inlineStr">
         <is>
-          <t>13001103</t>
+          <t>13001112</t>
         </is>
       </c>
     </row>
@@ -6906,12 +6906,12 @@
       </c>
       <c r="B382" t="inlineStr">
         <is>
-          <t>Пингвин</t>
+          <t>Classic Music HD</t>
         </is>
       </c>
       <c r="C382" t="inlineStr">
         <is>
-          <t>13001104</t>
+          <t>13001113</t>
         </is>
       </c>
     </row>
@@ -6923,12 +6923,12 @@
       </c>
       <c r="B383" t="inlineStr">
         <is>
-          <t>Еда</t>
+          <t>9 канал Израиль</t>
         </is>
       </c>
       <c r="C383" t="inlineStr">
         <is>
-          <t>13001105</t>
+          <t>13001118</t>
         </is>
       </c>
     </row>
@@ -6940,12 +6940,12 @@
       </c>
       <c r="B384" t="inlineStr">
         <is>
-          <t>Родное кино</t>
+          <t>Nicktoons</t>
         </is>
       </c>
       <c r="C384" t="inlineStr">
         <is>
-          <t>13001106</t>
+          <t>13001119</t>
         </is>
       </c>
     </row>
@@ -6957,12 +6957,12 @@
       </c>
       <c r="B385" t="inlineStr">
         <is>
-          <t>Кинохит HD</t>
+          <t>ТНТ Int</t>
         </is>
       </c>
       <c r="C385" t="inlineStr">
         <is>
-          <t>13001107</t>
+          <t>13001120</t>
         </is>
       </c>
     </row>
@@ -6974,12 +6974,12 @@
       </c>
       <c r="B386" t="inlineStr">
         <is>
-          <t>Зоо ТВ</t>
+          <t>Дорама HD</t>
         </is>
       </c>
       <c r="C386" t="inlineStr">
         <is>
-          <t>13001108</t>
+          <t>13001121</t>
         </is>
       </c>
     </row>
@@ -6991,12 +6991,12 @@
       </c>
       <c r="B387" t="inlineStr">
         <is>
-          <t>Balticum Platinum HD</t>
+          <t>Shot TV</t>
         </is>
       </c>
       <c r="C387" t="inlineStr">
         <is>
-          <t>13001109</t>
+          <t>13001122</t>
         </is>
       </c>
     </row>
@@ -7008,12 +7008,12 @@
       </c>
       <c r="B388" t="inlineStr">
         <is>
-          <t>Живи Активно HD</t>
+          <t>Filmbox</t>
         </is>
       </c>
       <c r="C388" t="inlineStr">
         <is>
-          <t>13001110</t>
+          <t>13001123</t>
         </is>
       </c>
     </row>
@@ -7025,12 +7025,12 @@
       </c>
       <c r="B389" t="inlineStr">
         <is>
-          <t>Живи! HD</t>
+          <t>Иллюзион+ HD</t>
         </is>
       </c>
       <c r="C389" t="inlineStr">
         <is>
-          <t>13001111</t>
+          <t>13001124</t>
         </is>
       </c>
     </row>
@@ -7042,12 +7042,12 @@
       </c>
       <c r="B390" t="inlineStr">
         <is>
-          <t>Карусель HD</t>
+          <t>К-Серия HD</t>
         </is>
       </c>
       <c r="C390" t="inlineStr">
         <is>
-          <t>13001112</t>
+          <t>13001125</t>
         </is>
       </c>
     </row>
@@ -7059,12 +7059,12 @@
       </c>
       <c r="B391" t="inlineStr">
         <is>
-          <t>Classic Music HD</t>
+          <t>AIVA HD</t>
         </is>
       </c>
       <c r="C391" t="inlineStr">
         <is>
-          <t>13001113</t>
+          <t>13001126</t>
         </is>
       </c>
     </row>
@@ -7076,12 +7076,12 @@
       </c>
       <c r="B392" t="inlineStr">
         <is>
-          <t>9 канал Израиль</t>
+          <t>MyZenTV HD</t>
         </is>
       </c>
       <c r="C392" t="inlineStr">
         <is>
-          <t>13001118</t>
+          <t>13001129</t>
         </is>
       </c>
     </row>
@@ -7093,12 +7093,12 @@
       </c>
       <c r="B393" t="inlineStr">
         <is>
-          <t>Nicktoons</t>
+          <t>MTV Live HD</t>
         </is>
       </c>
       <c r="C393" t="inlineStr">
         <is>
-          <t>13001119</t>
+          <t>13001133</t>
         </is>
       </c>
     </row>
@@ -7110,12 +7110,12 @@
       </c>
       <c r="B394" t="inlineStr">
         <is>
-          <t>ТНТ Int</t>
+          <t>Da Vinci</t>
         </is>
       </c>
       <c r="C394" t="inlineStr">
         <is>
-          <t>13001120</t>
+          <t>13001134</t>
         </is>
       </c>
     </row>
@@ -7127,12 +7127,12 @@
       </c>
       <c r="B395" t="inlineStr">
         <is>
-          <t>Дорама HD</t>
+          <t>А-Плюс HD</t>
         </is>
       </c>
       <c r="C395" t="inlineStr">
         <is>
-          <t>13001121</t>
+          <t>13001135</t>
         </is>
       </c>
     </row>
@@ -7144,12 +7144,12 @@
       </c>
       <c r="B396" t="inlineStr">
         <is>
-          <t>Shot TV</t>
+          <t>Кухня ТВ HD</t>
         </is>
       </c>
       <c r="C396" t="inlineStr">
         <is>
-          <t>13001122</t>
+          <t>13001137</t>
         </is>
       </c>
     </row>
@@ -7161,12 +7161,12 @@
       </c>
       <c r="B397" t="inlineStr">
         <is>
-          <t>Filmbox</t>
+          <t>Travel Channel HD</t>
         </is>
       </c>
       <c r="C397" t="inlineStr">
         <is>
-          <t>13001123</t>
+          <t>13001138</t>
         </is>
       </c>
     </row>
@@ -7178,12 +7178,12 @@
       </c>
       <c r="B398" t="inlineStr">
         <is>
-          <t>Иллюзион+ HD</t>
+          <t>Viva Russia HD</t>
         </is>
       </c>
       <c r="C398" t="inlineStr">
         <is>
-          <t>13001124</t>
+          <t>13001141</t>
         </is>
       </c>
     </row>
@@ -7195,12 +7195,12 @@
       </c>
       <c r="B399" t="inlineStr">
         <is>
-          <t>Киносерия HD</t>
+          <t>Hollywood HD</t>
         </is>
       </c>
       <c r="C399" t="inlineStr">
         <is>
-          <t>13001125</t>
+          <t>13001142</t>
         </is>
       </c>
     </row>
@@ -7212,12 +7212,12 @@
       </c>
       <c r="B400" t="inlineStr">
         <is>
-          <t>AIVA HD</t>
+          <t>Chiplduk Барбоскины</t>
         </is>
       </c>
       <c r="C400" t="inlineStr">
         <is>
-          <t>13001126</t>
+          <t>13001143</t>
         </is>
       </c>
     </row>
@@ -7229,12 +7229,12 @@
       </c>
       <c r="B401" t="inlineStr">
         <is>
-          <t>Epic Drama HD</t>
+          <t>C-Live HD</t>
         </is>
       </c>
       <c r="C401" t="inlineStr">
         <is>
-          <t>13001128</t>
+          <t>13001144</t>
         </is>
       </c>
     </row>
@@ -7246,12 +7246,12 @@
       </c>
       <c r="B402" t="inlineStr">
         <is>
-          <t>MyZenTV HD</t>
+          <t>Kernel TV За гранью HD</t>
         </is>
       </c>
       <c r="C402" t="inlineStr">
         <is>
-          <t>13001129</t>
+          <t>13001145</t>
         </is>
       </c>
     </row>
@@ -7263,12 +7263,12 @@
       </c>
       <c r="B403" t="inlineStr">
         <is>
-          <t>MTV Live HD</t>
+          <t>Kernel TV Сверхьестественное HD</t>
         </is>
       </c>
       <c r="C403" t="inlineStr">
         <is>
-          <t>13001133</t>
+          <t>13001146</t>
         </is>
       </c>
     </row>
@@ -7280,12 +7280,12 @@
       </c>
       <c r="B404" t="inlineStr">
         <is>
-          <t>Da Vinci</t>
+          <t>Kernel TV Во все тяжкие HD</t>
         </is>
       </c>
       <c r="C404" t="inlineStr">
         <is>
-          <t>13001134</t>
+          <t>13001147</t>
         </is>
       </c>
     </row>
@@ -7297,12 +7297,12 @@
       </c>
       <c r="B405" t="inlineStr">
         <is>
-          <t>АВТО Плюс HD</t>
+          <t>Kernel TV Бумажный дом HD</t>
         </is>
       </c>
       <c r="C405" t="inlineStr">
         <is>
-          <t>13001135</t>
+          <t>13001148</t>
         </is>
       </c>
     </row>
@@ -7314,12 +7314,12 @@
       </c>
       <c r="B406" t="inlineStr">
         <is>
-          <t>Кухня ТВ HD</t>
+          <t>Karloson TV Губка Боб HD</t>
         </is>
       </c>
       <c r="C406" t="inlineStr">
         <is>
-          <t>13001137</t>
+          <t>13001149</t>
         </is>
       </c>
     </row>
@@ -7331,12 +7331,12 @@
       </c>
       <c r="B407" t="inlineStr">
         <is>
-          <t>Travel Channel HD</t>
+          <t>Karloson TV Щенячий Патруль HD</t>
         </is>
       </c>
       <c r="C407" t="inlineStr">
         <is>
-          <t>13001138</t>
+          <t>13001150</t>
         </is>
       </c>
     </row>
@@ -7348,12 +7348,12 @@
       </c>
       <c r="B408" t="inlineStr">
         <is>
-          <t>Viva Russia HD</t>
+          <t>Karloson TV Интерны HD</t>
         </is>
       </c>
       <c r="C408" t="inlineStr">
         <is>
-          <t>13001141</t>
+          <t>13001151</t>
         </is>
       </c>
     </row>
@@ -7365,12 +7365,12 @@
       </c>
       <c r="B409" t="inlineStr">
         <is>
-          <t>Hollywood HD</t>
+          <t>Karloson TV My Little Pony HD</t>
         </is>
       </c>
       <c r="C409" t="inlineStr">
         <is>
-          <t>13001142</t>
+          <t>13001152</t>
         </is>
       </c>
     </row>
@@ -7382,12 +7382,12 @@
       </c>
       <c r="B410" t="inlineStr">
         <is>
-          <t>Chiplduk Барбоскины</t>
+          <t>Karloson TV Супер-крылья Джетт HD</t>
         </is>
       </c>
       <c r="C410" t="inlineStr">
         <is>
-          <t>13001143</t>
+          <t>13001153</t>
         </is>
       </c>
     </row>
@@ -7399,12 +7399,12 @@
       </c>
       <c r="B411" t="inlineStr">
         <is>
-          <t>C-Live HD</t>
+          <t>Karloson TV Утиные истории HD</t>
         </is>
       </c>
       <c r="C411" t="inlineStr">
         <is>
-          <t>13001144</t>
+          <t>13001154</t>
         </is>
       </c>
     </row>
@@ -7416,12 +7416,12 @@
       </c>
       <c r="B412" t="inlineStr">
         <is>
-          <t>Kernel TV За гранью HD</t>
+          <t>Karloson TV Симпсоны HD</t>
         </is>
       </c>
       <c r="C412" t="inlineStr">
         <is>
-          <t>13001145</t>
+          <t>13001155</t>
         </is>
       </c>
     </row>
@@ -7433,12 +7433,12 @@
       </c>
       <c r="B413" t="inlineStr">
         <is>
-          <t>Kernel TV Сверхьестественное HD</t>
+          <t>Karloson TV Чип и Дейл HD</t>
         </is>
       </c>
       <c r="C413" t="inlineStr">
         <is>
-          <t>13001146</t>
+          <t>13001156</t>
         </is>
       </c>
     </row>
@@ -7450,12 +7450,12 @@
       </c>
       <c r="B414" t="inlineStr">
         <is>
-          <t>Kernel TV Во все тяжкие HD</t>
+          <t>Karloson TV Южный Парк HD</t>
         </is>
       </c>
       <c r="C414" t="inlineStr">
         <is>
-          <t>13001147</t>
+          <t>13001157</t>
         </is>
       </c>
     </row>
@@ -7467,12 +7467,12 @@
       </c>
       <c r="B415" t="inlineStr">
         <is>
-          <t>Kernel TV Бумажный дом HD</t>
+          <t>М! Футбол 1 orig</t>
         </is>
       </c>
       <c r="C415" t="inlineStr">
         <is>
-          <t>13001148</t>
+          <t>13001158</t>
         </is>
       </c>
     </row>
@@ -7484,12 +7484,12 @@
       </c>
       <c r="B416" t="inlineStr">
         <is>
-          <t>Karloson TV Губка Боб HD</t>
+          <t>М! Футбол 2 orig</t>
         </is>
       </c>
       <c r="C416" t="inlineStr">
         <is>
-          <t>13001149</t>
+          <t>13001159</t>
         </is>
       </c>
     </row>
@@ -7501,12 +7501,12 @@
       </c>
       <c r="B417" t="inlineStr">
         <is>
-          <t>Karloson TV Щенячий Патруль HD</t>
+          <t>М! Футбол 3 orig</t>
         </is>
       </c>
       <c r="C417" t="inlineStr">
         <is>
-          <t>13001150</t>
+          <t>13001160</t>
         </is>
       </c>
     </row>
@@ -7518,12 +7518,12 @@
       </c>
       <c r="B418" t="inlineStr">
         <is>
-          <t>Karloson TV Интерны HD</t>
+          <t>М! orig</t>
         </is>
       </c>
       <c r="C418" t="inlineStr">
         <is>
-          <t>13001151</t>
+          <t>13001165</t>
         </is>
       </c>
     </row>
@@ -7535,12 +7535,12 @@
       </c>
       <c r="B419" t="inlineStr">
         <is>
-          <t>Karloson TV My Little Pony HD</t>
+          <t>М! Премьер orig</t>
         </is>
       </c>
       <c r="C419" t="inlineStr">
         <is>
-          <t>13001152</t>
+          <t>13001166</t>
         </is>
       </c>
     </row>
@@ -7552,12 +7552,12 @@
       </c>
       <c r="B420" t="inlineStr">
         <is>
-          <t>Karloson TV Супер-крылья Джетт HD</t>
+          <t>Kernel TV Буба HD</t>
         </is>
       </c>
       <c r="C420" t="inlineStr">
         <is>
-          <t>13001153</t>
+          <t>13001168</t>
         </is>
       </c>
     </row>
@@ -7569,12 +7569,12 @@
       </c>
       <c r="B421" t="inlineStr">
         <is>
-          <t>Karloson TV Утиные истории HD</t>
+          <t>Успех</t>
         </is>
       </c>
       <c r="C421" t="inlineStr">
         <is>
-          <t>13001154</t>
+          <t>13001169</t>
         </is>
       </c>
     </row>
@@ -7586,12 +7586,12 @@
       </c>
       <c r="B422" t="inlineStr">
         <is>
-          <t>Karloson TV Симпсоны HD</t>
+          <t>Охотник и Рыболов HD</t>
         </is>
       </c>
       <c r="C422" t="inlineStr">
         <is>
-          <t>13001155</t>
+          <t>13001170</t>
         </is>
       </c>
     </row>
@@ -7603,12 +7603,12 @@
       </c>
       <c r="B423" t="inlineStr">
         <is>
-          <t>Karloson TV Чип и Дейл HD</t>
+          <t>ducktv HD</t>
         </is>
       </c>
       <c r="C423" t="inlineStr">
         <is>
-          <t>13001156</t>
+          <t>13001173</t>
         </is>
       </c>
     </row>
@@ -7620,12 +7620,12 @@
       </c>
       <c r="B424" t="inlineStr">
         <is>
-          <t>Karloson TV Южный Парк HD</t>
+          <t>KIDS TV HD</t>
         </is>
       </c>
       <c r="C424" t="inlineStr">
         <is>
-          <t>13001157</t>
+          <t>13001174</t>
         </is>
       </c>
     </row>
@@ -7637,12 +7637,12 @@
       </c>
       <c r="B425" t="inlineStr">
         <is>
-          <t>М! Футбол 1 orig</t>
+          <t>CuriosityStream HD</t>
         </is>
       </c>
       <c r="C425" t="inlineStr">
         <is>
-          <t>13001158</t>
+          <t>13001175</t>
         </is>
       </c>
     </row>
@@ -7654,12 +7654,12 @@
       </c>
       <c r="B426" t="inlineStr">
         <is>
-          <t>М! Футбол 2 orig</t>
+          <t>Food Bloggers TV</t>
         </is>
       </c>
       <c r="C426" t="inlineStr">
         <is>
-          <t>13001159</t>
+          <t>13001176</t>
         </is>
       </c>
     </row>
@@ -7671,12 +7671,12 @@
       </c>
       <c r="B427" t="inlineStr">
         <is>
-          <t>М! Футбол 3 orig</t>
+          <t>Karloson TV Аладдин</t>
         </is>
       </c>
       <c r="C427" t="inlineStr">
         <is>
-          <t>13001160</t>
+          <t>13001197</t>
         </is>
       </c>
     </row>
@@ -7688,12 +7688,12 @@
       </c>
       <c r="B428" t="inlineStr">
         <is>
-          <t>Матч! orig</t>
+          <t>M2O</t>
         </is>
       </c>
       <c r="C428" t="inlineStr">
         <is>
-          <t>13001165</t>
+          <t>13001198</t>
         </is>
       </c>
     </row>
@@ -7705,12 +7705,12 @@
       </c>
       <c r="B429" t="inlineStr">
         <is>
-          <t>М! Премьер orig</t>
+          <t>Ritsa TV HD</t>
         </is>
       </c>
       <c r="C429" t="inlineStr">
         <is>
-          <t>13001166</t>
+          <t>13001199</t>
         </is>
       </c>
     </row>
@@ -7722,12 +7722,12 @@
       </c>
       <c r="B430" t="inlineStr">
         <is>
-          <t>Kernel TV Буба HD</t>
+          <t>Mafi2a Music</t>
         </is>
       </c>
       <c r="C430" t="inlineStr">
         <is>
-          <t>13001168</t>
+          <t>13001200</t>
         </is>
       </c>
     </row>
@@ -7739,12 +7739,12 @@
       </c>
       <c r="B431" t="inlineStr">
         <is>
-          <t>Успех</t>
+          <t>LO-FI Music Radio</t>
         </is>
       </c>
       <c r="C431" t="inlineStr">
         <is>
-          <t>13001169</t>
+          <t>13001201</t>
         </is>
       </c>
     </row>
@@ -7756,12 +7756,12 @@
       </c>
       <c r="B432" t="inlineStr">
         <is>
-          <t>Охотник и Рыболов HD</t>
+          <t>Полный Чипльдук</t>
         </is>
       </c>
       <c r="C432" t="inlineStr">
         <is>
-          <t>13001170</t>
+          <t>11000035</t>
         </is>
       </c>
     </row>
@@ -7773,12 +7773,12 @@
       </c>
       <c r="B433" t="inlineStr">
         <is>
-          <t>ducktv HD</t>
+          <t>Electro Swing Radio</t>
         </is>
       </c>
       <c r="C433" t="inlineStr">
         <is>
-          <t>13001173</t>
+          <t>11000041</t>
         </is>
       </c>
     </row>
@@ -7790,95 +7790,10 @@
       </c>
       <c r="B434" t="inlineStr">
         <is>
-          <t>KIDS TV HD</t>
+          <t>Локальный IGMP</t>
         </is>
       </c>
       <c r="C434" t="inlineStr">
-        <is>
-          <t>13001174</t>
-        </is>
-      </c>
-    </row>
-    <row r="435">
-      <c r="A435" t="inlineStr">
-        <is>
-          <t>433</t>
-        </is>
-      </c>
-      <c r="B435" t="inlineStr">
-        <is>
-          <t>CuriosityStream HD</t>
-        </is>
-      </c>
-      <c r="C435" t="inlineStr">
-        <is>
-          <t>13001175</t>
-        </is>
-      </c>
-    </row>
-    <row r="436">
-      <c r="A436" t="inlineStr">
-        <is>
-          <t>434</t>
-        </is>
-      </c>
-      <c r="B436" t="inlineStr">
-        <is>
-          <t>Food Bloggers TV</t>
-        </is>
-      </c>
-      <c r="C436" t="inlineStr">
-        <is>
-          <t>13001176</t>
-        </is>
-      </c>
-    </row>
-    <row r="437">
-      <c r="A437" t="inlineStr">
-        <is>
-          <t>435</t>
-        </is>
-      </c>
-      <c r="B437" t="inlineStr">
-        <is>
-          <t>Полный Чипльдук</t>
-        </is>
-      </c>
-      <c r="C437" t="inlineStr">
-        <is>
-          <t>11000035</t>
-        </is>
-      </c>
-    </row>
-    <row r="438">
-      <c r="A438" t="inlineStr">
-        <is>
-          <t>436</t>
-        </is>
-      </c>
-      <c r="B438" t="inlineStr">
-        <is>
-          <t>Electro Swing Radio</t>
-        </is>
-      </c>
-      <c r="C438" t="inlineStr">
-        <is>
-          <t>11000041</t>
-        </is>
-      </c>
-    </row>
-    <row r="439">
-      <c r="A439" t="inlineStr">
-        <is>
-          <t>437</t>
-        </is>
-      </c>
-      <c r="B439" t="inlineStr">
-        <is>
-          <t>Локальный IGMP</t>
-        </is>
-      </c>
-      <c r="C439" t="inlineStr">
         <is>
           <t>11000048</t>
         </is>

</xml_diff>

<commit_message>
Upload file 4duk_channels on 2023-10-20 21:11:26.767715
</commit_message>
<xml_diff>
--- a/4duk_channels.xlsx
+++ b/4duk_channels.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C434"/>
+  <dimension ref="A1:C435"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7756,12 +7756,12 @@
       </c>
       <c r="B432" t="inlineStr">
         <is>
-          <t>Полный Чипльдук</t>
+          <t>Santa</t>
         </is>
       </c>
       <c r="C432" t="inlineStr">
         <is>
-          <t>11000035</t>
+          <t>13001203</t>
         </is>
       </c>
     </row>
@@ -7773,12 +7773,12 @@
       </c>
       <c r="B433" t="inlineStr">
         <is>
-          <t>Electro Swing Radio</t>
+          <t>Полный Чипльдук</t>
         </is>
       </c>
       <c r="C433" t="inlineStr">
         <is>
-          <t>11000041</t>
+          <t>11000035</t>
         </is>
       </c>
     </row>
@@ -7790,10 +7790,27 @@
       </c>
       <c r="B434" t="inlineStr">
         <is>
+          <t>Electro Swing Radio</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>11000041</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>433</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
           <t>Локальный IGMP</t>
         </is>
       </c>
-      <c r="C434" t="inlineStr">
+      <c r="C435" t="inlineStr">
         <is>
           <t>11000048</t>
         </is>

</xml_diff>